<commit_message>
Mise à jour du MCD
</commit_message>
<xml_diff>
--- a/conception/MCD/Dictionnaire de données -P-MCD.xlsx
+++ b/conception/MCD/Dictionnaire de données -P-MCD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\#AFPACAR\MCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_AFPACAR\projet_afpa_car\conception\MCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>Modèle de dictionnaire de données</t>
   </si>
@@ -44,223 +44,217 @@
     <t>AFPA CAR</t>
   </si>
   <si>
-    <t>Utilisateur</t>
-  </si>
-  <si>
-    <t>nom_utilisateur</t>
-  </si>
-  <si>
-    <t>prenom_utilisateur</t>
-  </si>
-  <si>
-    <t>mail</t>
-  </si>
-  <si>
-    <t>telephone</t>
-  </si>
-  <si>
-    <t>permis</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>AN</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>non null</t>
-  </si>
-  <si>
-    <t>Vehicule</t>
-  </si>
-  <si>
-    <t>modele</t>
-  </si>
-  <si>
-    <t>consommation</t>
-  </si>
-  <si>
-    <t>carburant</t>
-  </si>
-  <si>
-    <t>(essence/gasoil/electrique)</t>
-  </si>
-  <si>
-    <t>conducteur</t>
-  </si>
-  <si>
-    <t>Trajet</t>
-  </si>
-  <si>
-    <t>heure_depart_matin</t>
-  </si>
-  <si>
-    <t>heure_arrivee_matin</t>
-  </si>
-  <si>
-    <t>heure_depart_soir</t>
-  </si>
-  <si>
-    <t>Point rencontre</t>
-  </si>
-  <si>
-    <t>fumeur</t>
-  </si>
-  <si>
     <t>Conversation</t>
   </si>
   <si>
-    <t>mot_de_passe</t>
-  </si>
-  <si>
-    <t>code_postal</t>
-  </si>
-  <si>
-    <t>rue</t>
-  </si>
-  <si>
-    <t>numero_rue</t>
-  </si>
-  <si>
-    <t>ville</t>
-  </si>
-  <si>
-    <t>Centre_AFPA</t>
-  </si>
-  <si>
-    <t>Adresses(utilisateurs/centre_AFPA/points rencontre)</t>
-  </si>
-  <si>
     <t>Formation</t>
   </si>
   <si>
-    <t>date_debut_stage</t>
-  </si>
-  <si>
-    <t>date_fin_stage</t>
-  </si>
-  <si>
-    <t>identifiant_afpa</t>
-  </si>
-  <si>
-    <t>Jour</t>
-  </si>
-  <si>
-    <t>nom_jour</t>
-  </si>
-  <si>
-    <t>nombre_places_vehicule</t>
-  </si>
-  <si>
-    <t>Trajet_type</t>
-  </si>
-  <si>
-    <t>stagiaire/employé</t>
-  </si>
-  <si>
-    <t>Nom_centre</t>
-  </si>
-  <si>
-    <t>couleur</t>
-  </si>
-  <si>
-    <t>pseudo</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
     <t>longitude</t>
   </si>
   <si>
-    <t>numero_immatriculation</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>heure_arrivee_soir_estimee</t>
-  </si>
-  <si>
-    <t>id_conversation</t>
-  </si>
-  <si>
-    <t>Session de Formation</t>
-  </si>
-  <si>
-    <t>date_début_formation</t>
-  </si>
-  <si>
-    <t>date_fin_formation</t>
-  </si>
-  <si>
     <t>Message</t>
   </si>
   <si>
-    <t>contenu_message</t>
-  </si>
-  <si>
-    <t>libelle_formation</t>
-  </si>
-  <si>
-    <t>avatar</t>
-  </si>
-  <si>
-    <t>URL/Img</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Datetime</t>
-  </si>
-  <si>
-    <t>estimation_cout_trajet</t>
-  </si>
-  <si>
-    <t>calculé</t>
-  </si>
-  <si>
-    <t>facultatif</t>
-  </si>
-  <si>
-    <t>conso*longueur_trajet*prix_carburant</t>
-  </si>
-  <si>
-    <t>libelle</t>
-  </si>
-  <si>
-    <t>complement_adresse</t>
-  </si>
-  <si>
-    <t>Donnees personnelles</t>
-  </si>
-  <si>
-    <t>Ville</t>
-  </si>
-  <si>
-    <t>nom_ville</t>
-  </si>
-  <si>
-    <t>Code_postal</t>
-  </si>
-  <si>
-    <t>numero_code_postal</t>
-  </si>
-  <si>
-    <t>prive_ou_public</t>
-  </si>
-  <si>
     <t>Bool</t>
   </si>
   <si>
-    <t>Hérite de trajet_type</t>
+    <t>User</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Varchar (50)</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>is_staff</t>
+  </si>
+  <si>
+    <t>is_admin</t>
+  </si>
+  <si>
+    <t>date_joined</t>
+  </si>
+  <si>
+    <t>confirm</t>
+  </si>
+  <si>
+    <t>confirmation_date</t>
+  </si>
+  <si>
+    <t>UserProfile</t>
+  </si>
+  <si>
+    <t>driver_license</t>
+  </si>
+  <si>
+    <t>trainee</t>
+  </si>
+  <si>
+    <t>car_owner</t>
+  </si>
+  <si>
+    <t>profile_image</t>
+  </si>
+  <si>
+    <t>Varchar (20)</t>
+  </si>
+  <si>
+    <t>smoker</t>
+  </si>
+  <si>
+    <t>talker</t>
+  </si>
+  <si>
+    <t>music</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>PrivateData</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>afpa_number</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>amount_of_free_seats</t>
+  </si>
+  <si>
+    <t>Int</t>
+  </si>
+  <si>
+    <t>consumption</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>FormationSession</t>
+  </si>
+  <si>
+    <t>formation_session_start_date</t>
+  </si>
+  <si>
+    <t>formation_session_end_date</t>
+  </si>
+  <si>
+    <t>work_experience_end_date</t>
+  </si>
+  <si>
+    <t>work_experience_start_date</t>
+  </si>
+  <si>
+    <t>formation_name</t>
+  </si>
+  <si>
+    <t>Varchar(50)</t>
+  </si>
+  <si>
+    <t>AfpaCenter</t>
+  </si>
+  <si>
+    <t>center_name</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>zip_code</t>
+  </si>
+  <si>
+    <t>street_name</t>
+  </si>
+  <si>
+    <t>street_number</t>
+  </si>
+  <si>
+    <t>national_reference</t>
+  </si>
+  <si>
+    <t>adress_label</t>
+  </si>
+  <si>
+    <t>MeetingPoint</t>
+  </si>
+  <si>
+    <t>public_or_private</t>
+  </si>
+  <si>
+    <t>DefaultTrip</t>
+  </si>
+  <si>
+    <t>morning_departure_time</t>
+  </si>
+  <si>
+    <t>morning_arriving_time</t>
+  </si>
+  <si>
+    <t>evening_departure_time</t>
+  </si>
+  <si>
+    <t>estimated_trip_cost</t>
+  </si>
+  <si>
+    <t>Fonction des données de la voiture et de la longueur du trajet</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>day_name</t>
+  </si>
+  <si>
+    <t>Trip</t>
+  </si>
+  <si>
+    <t>trip_date</t>
+  </si>
+  <si>
+    <t>message_content</t>
+  </si>
+  <si>
+    <t>Varchar (500)</t>
   </si>
 </sst>
 </file>
@@ -463,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -490,13 +484,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -534,11 +521,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -555,36 +560,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,28 +847,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P751"/>
+  <dimension ref="B1:P760"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:16" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -915,95 +896,87 @@
       </c>
     </row>
     <row r="3" spans="2:16" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
     </row>
     <row r="4" spans="2:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="B4" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
     </row>
     <row r="5" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="9"/>
     </row>
     <row r="7" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="9" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="9"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1013,587 +986,563 @@
         <v>22</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="41" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
-        <v>10</v>
-      </c>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="44"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="16"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="16"/>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="16"/>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+    </row>
+    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="29"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="37"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="38"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+    </row>
+    <row r="43" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="32"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+    </row>
+    <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="37"/>
+      <c r="D44" s="37"/>
+      <c r="E44" s="38"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="23"/>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="14"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="15"/>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="38"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+    </row>
+    <row r="49" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="9"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="38"/>
+    </row>
+    <row r="51" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="17"/>
+    </row>
+    <row r="52" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="18"/>
+    </row>
+    <row r="53" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="18"/>
+    </row>
+    <row r="54" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="18"/>
+    </row>
+    <row r="55" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C55" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="18"/>
+    </row>
+    <row r="56" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="18"/>
+    </row>
+    <row r="57" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="44"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="33" t="s">
+      <c r="C57" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="18"/>
+    </row>
+    <row r="58" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="4"/>
+      <c r="E58" s="18"/>
+    </row>
+    <row r="59" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="32"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="34"/>
+    </row>
+    <row r="60" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="38"/>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="19"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="19"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="19"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="19"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="19"/>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="19"/>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="19"/>
-    </row>
-    <row r="29" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="41" t="s">
-        <v>72</v>
-      </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="25"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-    </row>
-    <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="32"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-    </row>
-    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="43"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-    </row>
-    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="45"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-    </row>
-    <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="26"/>
-    </row>
-    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="17"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="18"/>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="43"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="4"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="4"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="4"/>
-    </row>
-    <row r="42" spans="2:5" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="14"/>
-    </row>
-    <row r="43" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" s="12"/>
-    </row>
-    <row r="44" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="12"/>
-    </row>
-    <row r="45" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="C45" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-    </row>
-    <row r="46" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="9"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-    </row>
-    <row r="47" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="C47" s="42"/>
-      <c r="D47" s="42"/>
-      <c r="E47" s="43"/>
-    </row>
-    <row r="48" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="C48" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E48" s="20"/>
-    </row>
-    <row r="49" spans="2:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="50"/>
-    </row>
-    <row r="50" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="45"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="47"/>
-    </row>
-    <row r="51" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="42"/>
-      <c r="D51" s="42"/>
-      <c r="E51" s="43"/>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="29" t="s">
+      <c r="D61" s="26"/>
+      <c r="E61" s="29"/>
+    </row>
+    <row r="62" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="9"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+    </row>
+    <row r="63" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D52" s="29" t="s">
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="38"/>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E52" s="32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="9"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="C58" s="42"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="43"/>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="4"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="41" t="s">
-        <v>29</v>
-      </c>
-      <c r="C61" s="42"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="43"/>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="4"/>
-    </row>
-    <row r="63" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="9"/>
-      <c r="C63" s="6"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-    </row>
-    <row r="64" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C64" s="42"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="43"/>
+      <c r="C64" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D65" s="4"/>
       <c r="E65" s="4"/>
     </row>
-    <row r="66" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="4"/>
-      <c r="C66" s="6"/>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
     </row>
-    <row r="67" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="C67" s="42"/>
-      <c r="D67" s="42"/>
-      <c r="E67" s="43"/>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E68" s="30"/>
+      <c r="B68" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="69" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="22"/>
-      <c r="C69" s="23"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-    </row>
-    <row r="70" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C70" s="42"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="43"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+    </row>
+    <row r="70" spans="2:5" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="38"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>16</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D71" s="4"/>
       <c r="E71" s="4"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B72" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>16</v>
-      </c>
+    <row r="72" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="9"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="4"/>
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
+    <row r="73" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="C73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="38"/>
     </row>
     <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -1605,40 +1554,40 @@
       <c r="E75" s="4"/>
     </row>
     <row r="76" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="C76" s="42"/>
-      <c r="D76" s="42"/>
-      <c r="E76" s="43"/>
+      <c r="B76" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="38"/>
     </row>
     <row r="77" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B77" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E77" s="4"/>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-      <c r="C78" s="6"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="28"/>
-      <c r="C79" s="28"/>
-      <c r="D79" s="28"/>
-      <c r="E79" s="28"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="27"/>
+    </row>
+    <row r="78" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="19"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+    </row>
+    <row r="79" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="38"/>
     </row>
     <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
-      <c r="C80" s="6"/>
+      <c r="B80" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
     </row>
@@ -1648,29 +1597,29 @@
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B82" s="4"/>
-      <c r="C82" s="13"/>
-      <c r="D82" s="13"/>
-      <c r="E82" s="13"/>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" s="9"/>
+      <c r="C82" s="6"/>
+      <c r="D82" s="4"/>
+      <c r="E82" s="4"/>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
+      <c r="B83" s="9"/>
       <c r="C83" s="6"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B84" s="4"/>
       <c r="C84" s="6"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
+    <row r="85" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="36"/>
+      <c r="C85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="38"/>
     </row>
     <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" s="4"/>
@@ -1685,10 +1634,10 @@
       <c r="E87" s="4"/>
     </row>
     <row r="88" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
-      <c r="C88" s="6"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
     </row>
     <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" s="4"/>
@@ -1697,19 +1646,19 @@
       <c r="E89" s="4"/>
     </row>
     <row r="90" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
+      <c r="B90" s="9"/>
       <c r="C90" s="6"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B91" s="4"/>
-      <c r="C91" s="6"/>
-      <c r="D91" s="4"/>
-      <c r="E91" s="4"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
     </row>
     <row r="92" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
+      <c r="B92" s="4"/>
       <c r="C92" s="6"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -1727,13 +1676,13 @@
       <c r="E94" s="4"/>
     </row>
     <row r="95" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B95" s="3"/>
+      <c r="B95" s="4"/>
       <c r="C95" s="6"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
     </row>
     <row r="96" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+      <c r="B96" s="3"/>
       <c r="C96" s="6"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -1762,14 +1711,14 @@
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
     </row>
-    <row r="101" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B101" s="13"/>
-      <c r="C101" s="13"/>
-      <c r="D101" s="13"/>
-      <c r="E101" s="13"/>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B101" s="3"/>
+      <c r="C101" s="6"/>
+      <c r="D101" s="4"/>
+      <c r="E101" s="4"/>
     </row>
     <row r="102" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
+      <c r="B102" s="4"/>
       <c r="C102" s="6"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -1781,7 +1730,7 @@
       <c r="E103" s="4"/>
     </row>
     <row r="104" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
+      <c r="B104" s="3"/>
       <c r="C104" s="6"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -1811,19 +1760,19 @@
       <c r="E108" s="4"/>
     </row>
     <row r="109" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B109" s="3"/>
+      <c r="B109" s="4"/>
       <c r="C109" s="6"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
-      <c r="C110" s="6"/>
-      <c r="D110" s="4"/>
-      <c r="E110" s="4"/>
+    <row r="110" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
     </row>
     <row r="111" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B111" s="4"/>
+      <c r="B111" s="3"/>
       <c r="C111" s="6"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -1835,7 +1784,7 @@
       <c r="E112" s="4"/>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B113" s="3"/>
+      <c r="B113" s="4"/>
       <c r="C113" s="6"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -1889,13 +1838,13 @@
       <c r="E121" s="4"/>
     </row>
     <row r="122" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B122" s="4"/>
+      <c r="B122" s="3"/>
       <c r="C122" s="6"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
     </row>
     <row r="123" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B123" s="3"/>
+      <c r="B123" s="4"/>
       <c r="C123" s="6"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
@@ -1918,14 +1867,14 @@
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
     </row>
-    <row r="127" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B127" s="13"/>
-      <c r="C127" s="13"/>
-      <c r="D127" s="13"/>
-      <c r="E127" s="13"/>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127" s="3"/>
+      <c r="C127" s="6"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="4"/>
     </row>
     <row r="128" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B128" s="3"/>
+      <c r="B128" s="4"/>
       <c r="C128" s="6"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -1949,7 +1898,7 @@
       <c r="E131" s="4"/>
     </row>
     <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="4"/>
+      <c r="B132" s="3"/>
       <c r="C132" s="6"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -1961,25 +1910,25 @@
       <c r="E133" s="4"/>
     </row>
     <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="3"/>
+      <c r="B134" s="4"/>
       <c r="C134" s="6"/>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
     </row>
     <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="9"/>
+      <c r="B135" s="4"/>
       <c r="C135" s="6"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="4"/>
-      <c r="C136" s="6"/>
-      <c r="D136" s="4"/>
-      <c r="E136" s="4"/>
+    <row r="136" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B136" s="13"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
     </row>
     <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="4"/>
+      <c r="B137" s="3"/>
       <c r="C137" s="6"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -1997,7 +1946,7 @@
       <c r="E139" s="4"/>
     </row>
     <row r="140" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B140" s="3"/>
+      <c r="B140" s="4"/>
       <c r="C140" s="6"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
@@ -2021,7 +1970,7 @@
       <c r="E143" s="4"/>
     </row>
     <row r="144" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B144" s="4"/>
+      <c r="B144" s="9"/>
       <c r="C144" s="6"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
@@ -2051,7 +2000,7 @@
       <c r="E148" s="4"/>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B149" s="4"/>
+      <c r="B149" s="3"/>
       <c r="C149" s="6"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
@@ -2069,7 +2018,7 @@
       <c r="E151" s="4"/>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B152" s="4"/>
+      <c r="B152" s="3"/>
       <c r="C152" s="6"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
@@ -2123,7 +2072,7 @@
       <c r="E160" s="4"/>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B161" s="3"/>
+      <c r="B161" s="4"/>
       <c r="C161" s="6"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
@@ -2171,13 +2120,13 @@
       <c r="E168" s="4"/>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B169" s="3"/>
+      <c r="B169" s="4"/>
       <c r="C169" s="6"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B170" s="4"/>
+      <c r="B170" s="3"/>
       <c r="C170" s="6"/>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
@@ -2218,11 +2167,11 @@
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
     </row>
-    <row r="177" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B177" s="40"/>
-      <c r="C177" s="40"/>
-      <c r="D177" s="40"/>
-      <c r="E177" s="40"/>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B177" s="4"/>
+      <c r="C177" s="6"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
     </row>
     <row r="178" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B178" s="3"/>
@@ -2267,25 +2216,25 @@
       <c r="E184" s="4"/>
     </row>
     <row r="185" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B185" s="3"/>
+      <c r="B185" s="4"/>
       <c r="C185" s="6"/>
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
     </row>
-    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B186" s="4"/>
-      <c r="C186" s="6"/>
-      <c r="D186" s="4"/>
-      <c r="E186" s="4"/>
+    <row r="186" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B186" s="43"/>
+      <c r="C186" s="43"/>
+      <c r="D186" s="43"/>
+      <c r="E186" s="43"/>
     </row>
     <row r="187" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B187" s="4"/>
+      <c r="B187" s="3"/>
       <c r="C187" s="6"/>
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
     </row>
     <row r="188" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B188" s="3"/>
+      <c r="B188" s="4"/>
       <c r="C188" s="6"/>
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
@@ -2303,7 +2252,7 @@
       <c r="E190" s="4"/>
     </row>
     <row r="191" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B191" s="3"/>
+      <c r="B191" s="4"/>
       <c r="C191" s="6"/>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
@@ -2321,7 +2270,7 @@
       <c r="E193" s="4"/>
     </row>
     <row r="194" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B194" s="4"/>
+      <c r="B194" s="3"/>
       <c r="C194" s="6"/>
       <c r="D194" s="4"/>
       <c r="E194" s="4"/>
@@ -2333,13 +2282,13 @@
       <c r="E195" s="4"/>
     </row>
     <row r="196" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B196" s="3"/>
+      <c r="B196" s="4"/>
       <c r="C196" s="6"/>
       <c r="D196" s="4"/>
       <c r="E196" s="4"/>
     </row>
     <row r="197" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B197" s="4"/>
+      <c r="B197" s="3"/>
       <c r="C197" s="6"/>
       <c r="D197" s="4"/>
       <c r="E197" s="4"/>
@@ -2375,7 +2324,7 @@
       <c r="E202" s="4"/>
     </row>
     <row r="203" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B203" s="3"/>
+      <c r="B203" s="4"/>
       <c r="C203" s="6"/>
       <c r="D203" s="4"/>
       <c r="E203" s="4"/>
@@ -2387,13 +2336,13 @@
       <c r="E204" s="4"/>
     </row>
     <row r="205" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B205" s="4"/>
+      <c r="B205" s="3"/>
       <c r="C205" s="6"/>
       <c r="D205" s="4"/>
       <c r="E205" s="4"/>
     </row>
     <row r="206" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B206" s="3"/>
+      <c r="B206" s="4"/>
       <c r="C206" s="6"/>
       <c r="D206" s="4"/>
       <c r="E206" s="4"/>
@@ -2446,14 +2395,14 @@
       <c r="D214" s="4"/>
       <c r="E214" s="4"/>
     </row>
-    <row r="215" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B215" s="40"/>
-      <c r="C215" s="40"/>
-      <c r="D215" s="40"/>
-      <c r="E215" s="40"/>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B215" s="3"/>
+      <c r="C215" s="6"/>
+      <c r="D215" s="4"/>
+      <c r="E215" s="4"/>
     </row>
     <row r="216" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B216" s="3"/>
+      <c r="B216" s="4"/>
       <c r="C216" s="6"/>
       <c r="D216" s="4"/>
       <c r="E216" s="4"/>
@@ -2465,7 +2414,7 @@
       <c r="E217" s="4"/>
     </row>
     <row r="218" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B218" s="4"/>
+      <c r="B218" s="3"/>
       <c r="C218" s="6"/>
       <c r="D218" s="4"/>
       <c r="E218" s="4"/>
@@ -2483,13 +2432,13 @@
       <c r="E220" s="4"/>
     </row>
     <row r="221" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B221" s="4"/>
+      <c r="B221" s="3"/>
       <c r="C221" s="6"/>
       <c r="D221" s="4"/>
       <c r="E221" s="4"/>
     </row>
     <row r="222" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B222" s="3"/>
+      <c r="B222" s="4"/>
       <c r="C222" s="6"/>
       <c r="D222" s="4"/>
       <c r="E222" s="4"/>
@@ -2500,20 +2449,20 @@
       <c r="D223" s="4"/>
       <c r="E223" s="4"/>
     </row>
-    <row r="224" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B224" s="4"/>
-      <c r="C224" s="6"/>
-      <c r="D224" s="4"/>
-      <c r="E224" s="4"/>
+    <row r="224" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B224" s="43"/>
+      <c r="C224" s="43"/>
+      <c r="D224" s="43"/>
+      <c r="E224" s="43"/>
     </row>
     <row r="225" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B225" s="4"/>
+      <c r="B225" s="3"/>
       <c r="C225" s="6"/>
       <c r="D225" s="4"/>
       <c r="E225" s="4"/>
     </row>
     <row r="226" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B226" s="3"/>
+      <c r="B226" s="4"/>
       <c r="C226" s="6"/>
       <c r="D226" s="4"/>
       <c r="E226" s="4"/>
@@ -2567,13 +2516,13 @@
       <c r="E234" s="4"/>
     </row>
     <row r="235" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B235" s="4"/>
+      <c r="B235" s="3"/>
       <c r="C235" s="6"/>
       <c r="D235" s="4"/>
       <c r="E235" s="4"/>
     </row>
     <row r="236" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B236" s="3"/>
+      <c r="B236" s="4"/>
       <c r="C236" s="6"/>
       <c r="D236" s="4"/>
       <c r="E236" s="4"/>
@@ -2597,7 +2546,7 @@
       <c r="E239" s="4"/>
     </row>
     <row r="240" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B240" s="4"/>
+      <c r="B240" s="3"/>
       <c r="C240" s="6"/>
       <c r="D240" s="4"/>
       <c r="E240" s="4"/>
@@ -2608,14 +2557,14 @@
       <c r="D241" s="4"/>
       <c r="E241" s="4"/>
     </row>
-    <row r="242" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B242" s="40"/>
-      <c r="C242" s="40"/>
-      <c r="D242" s="40"/>
-      <c r="E242" s="40"/>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B242" s="4"/>
+      <c r="C242" s="6"/>
+      <c r="D242" s="4"/>
+      <c r="E242" s="4"/>
     </row>
     <row r="243" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B243" s="3"/>
+      <c r="B243" s="4"/>
       <c r="C243" s="6"/>
       <c r="D243" s="4"/>
       <c r="E243" s="4"/>
@@ -2627,7 +2576,7 @@
       <c r="E244" s="4"/>
     </row>
     <row r="245" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B245" s="4"/>
+      <c r="B245" s="3"/>
       <c r="C245" s="6"/>
       <c r="D245" s="4"/>
       <c r="E245" s="4"/>
@@ -2657,19 +2606,19 @@
       <c r="E249" s="4"/>
     </row>
     <row r="250" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B250" s="3"/>
+      <c r="B250" s="4"/>
       <c r="C250" s="6"/>
       <c r="D250" s="4"/>
       <c r="E250" s="4"/>
     </row>
-    <row r="251" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B251" s="4"/>
-      <c r="C251" s="6"/>
-      <c r="D251" s="4"/>
-      <c r="E251" s="4"/>
+    <row r="251" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B251" s="43"/>
+      <c r="C251" s="43"/>
+      <c r="D251" s="43"/>
+      <c r="E251" s="43"/>
     </row>
     <row r="252" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B252" s="4"/>
+      <c r="B252" s="3"/>
       <c r="C252" s="6"/>
       <c r="D252" s="4"/>
       <c r="E252" s="4"/>
@@ -2711,13 +2660,13 @@
       <c r="E258" s="4"/>
     </row>
     <row r="259" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B259" s="4"/>
+      <c r="B259" s="3"/>
       <c r="C259" s="6"/>
       <c r="D259" s="4"/>
       <c r="E259" s="4"/>
     </row>
     <row r="260" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B260" s="3"/>
+      <c r="B260" s="4"/>
       <c r="C260" s="6"/>
       <c r="D260" s="4"/>
       <c r="E260" s="4"/>
@@ -2741,7 +2690,7 @@
       <c r="E263" s="4"/>
     </row>
     <row r="264" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B264" s="3"/>
+      <c r="B264" s="4"/>
       <c r="C264" s="6"/>
       <c r="D264" s="4"/>
       <c r="E264" s="4"/>
@@ -2759,7 +2708,7 @@
       <c r="E266" s="4"/>
     </row>
     <row r="267" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B267" s="3"/>
+      <c r="B267" s="4"/>
       <c r="C267" s="6"/>
       <c r="D267" s="4"/>
       <c r="E267" s="4"/>
@@ -2771,7 +2720,7 @@
       <c r="E268" s="4"/>
     </row>
     <row r="269" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B269" s="4"/>
+      <c r="B269" s="3"/>
       <c r="C269" s="6"/>
       <c r="D269" s="4"/>
       <c r="E269" s="4"/>
@@ -2789,13 +2738,13 @@
       <c r="E271" s="4"/>
     </row>
     <row r="272" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B272" s="3"/>
+      <c r="B272" s="4"/>
       <c r="C272" s="6"/>
       <c r="D272" s="4"/>
       <c r="E272" s="4"/>
     </row>
     <row r="273" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B273" s="4"/>
+      <c r="B273" s="3"/>
       <c r="C273" s="6"/>
       <c r="D273" s="4"/>
       <c r="E273" s="4"/>
@@ -2813,25 +2762,25 @@
       <c r="E275" s="4"/>
     </row>
     <row r="276" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B276" s="4"/>
+      <c r="B276" s="3"/>
       <c r="C276" s="6"/>
       <c r="D276" s="4"/>
       <c r="E276" s="4"/>
     </row>
-    <row r="277" spans="2:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="B277" s="40"/>
-      <c r="C277" s="40"/>
-      <c r="D277" s="40"/>
-      <c r="E277" s="40"/>
+    <row r="277" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B277" s="4"/>
+      <c r="C277" s="6"/>
+      <c r="D277" s="4"/>
+      <c r="E277" s="4"/>
     </row>
     <row r="278" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B278" s="3"/>
+      <c r="B278" s="4"/>
       <c r="C278" s="6"/>
       <c r="D278" s="4"/>
       <c r="E278" s="4"/>
     </row>
     <row r="279" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B279" s="9"/>
+      <c r="B279" s="4"/>
       <c r="C279" s="6"/>
       <c r="D279" s="4"/>
       <c r="E279" s="4"/>
@@ -2867,25 +2816,25 @@
       <c r="E284" s="4"/>
     </row>
     <row r="285" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B285" s="3"/>
+      <c r="B285" s="4"/>
       <c r="C285" s="6"/>
       <c r="D285" s="4"/>
       <c r="E285" s="4"/>
     </row>
-    <row r="286" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B286" s="9"/>
-      <c r="C286" s="6"/>
-      <c r="D286" s="4"/>
-      <c r="E286" s="4"/>
+    <row r="286" spans="2:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="B286" s="43"/>
+      <c r="C286" s="43"/>
+      <c r="D286" s="43"/>
+      <c r="E286" s="43"/>
     </row>
     <row r="287" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B287" s="4"/>
+      <c r="B287" s="3"/>
       <c r="C287" s="6"/>
       <c r="D287" s="4"/>
       <c r="E287" s="4"/>
     </row>
     <row r="288" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B288" s="4"/>
+      <c r="B288" s="9"/>
       <c r="C288" s="6"/>
       <c r="D288" s="4"/>
       <c r="E288" s="4"/>
@@ -2897,7 +2846,7 @@
       <c r="E289" s="4"/>
     </row>
     <row r="290" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B290" s="4"/>
+      <c r="B290" s="3"/>
       <c r="C290" s="6"/>
       <c r="D290" s="4"/>
       <c r="E290" s="4"/>
@@ -2909,7 +2858,7 @@
       <c r="E291" s="4"/>
     </row>
     <row r="292" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B292" s="3"/>
+      <c r="B292" s="4"/>
       <c r="C292" s="6"/>
       <c r="D292" s="4"/>
       <c r="E292" s="4"/>
@@ -2921,19 +2870,19 @@
       <c r="E293" s="4"/>
     </row>
     <row r="294" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B294" s="4"/>
+      <c r="B294" s="3"/>
       <c r="C294" s="6"/>
       <c r="D294" s="4"/>
       <c r="E294" s="4"/>
     </row>
     <row r="295" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B295" s="4"/>
+      <c r="B295" s="9"/>
       <c r="C295" s="6"/>
       <c r="D295" s="4"/>
       <c r="E295" s="4"/>
     </row>
     <row r="296" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B296" s="3"/>
+      <c r="B296" s="4"/>
       <c r="C296" s="6"/>
       <c r="D296" s="4"/>
       <c r="E296" s="4"/>
@@ -2957,13 +2906,13 @@
       <c r="E299" s="4"/>
     </row>
     <row r="300" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B300" s="3"/>
+      <c r="B300" s="4"/>
       <c r="C300" s="6"/>
       <c r="D300" s="4"/>
       <c r="E300" s="4"/>
     </row>
     <row r="301" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B301" s="4"/>
+      <c r="B301" s="3"/>
       <c r="C301" s="6"/>
       <c r="D301" s="4"/>
       <c r="E301" s="4"/>
@@ -2987,7 +2936,7 @@
       <c r="E304" s="4"/>
     </row>
     <row r="305" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B305" s="4"/>
+      <c r="B305" s="3"/>
       <c r="C305" s="6"/>
       <c r="D305" s="4"/>
       <c r="E305" s="4"/>
@@ -3011,7 +2960,7 @@
       <c r="E308" s="4"/>
     </row>
     <row r="309" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B309" s="4"/>
+      <c r="B309" s="3"/>
       <c r="C309" s="6"/>
       <c r="D309" s="4"/>
       <c r="E309" s="4"/>
@@ -5668,30 +5617,83 @@
       <c r="D751" s="4"/>
       <c r="E751" s="4"/>
     </row>
+    <row r="752" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B752" s="4"/>
+      <c r="C752" s="6"/>
+      <c r="D752" s="4"/>
+      <c r="E752" s="4"/>
+    </row>
+    <row r="753" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B753" s="4"/>
+      <c r="C753" s="6"/>
+      <c r="D753" s="4"/>
+      <c r="E753" s="4"/>
+    </row>
+    <row r="754" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B754" s="4"/>
+      <c r="C754" s="6"/>
+      <c r="D754" s="4"/>
+      <c r="E754" s="4"/>
+    </row>
+    <row r="755" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B755" s="4"/>
+      <c r="C755" s="6"/>
+      <c r="D755" s="4"/>
+      <c r="E755" s="4"/>
+    </row>
+    <row r="756" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B756" s="4"/>
+      <c r="C756" s="6"/>
+      <c r="D756" s="4"/>
+      <c r="E756" s="4"/>
+    </row>
+    <row r="757" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B757" s="4"/>
+      <c r="C757" s="6"/>
+      <c r="D757" s="4"/>
+      <c r="E757" s="4"/>
+    </row>
+    <row r="758" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B758" s="4"/>
+      <c r="C758" s="6"/>
+      <c r="D758" s="4"/>
+      <c r="E758" s="4"/>
+    </row>
+    <row r="759" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B759" s="4"/>
+      <c r="C759" s="6"/>
+      <c r="D759" s="4"/>
+      <c r="E759" s="4"/>
+    </row>
+    <row r="760" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B760" s="4"/>
+      <c r="C760" s="6"/>
+      <c r="D760" s="4"/>
+      <c r="E760" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="B32:E32"/>
-    <mergeCell ref="B49:E49"/>
+  <mergeCells count="21">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B215:E215"/>
-    <mergeCell ref="B242:E242"/>
-    <mergeCell ref="B277:E277"/>
-    <mergeCell ref="B177:E177"/>
+    <mergeCell ref="B224:E224"/>
+    <mergeCell ref="B251:E251"/>
+    <mergeCell ref="B286:E286"/>
+    <mergeCell ref="B186:E186"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B30:E30"/>
     <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="B61:E61"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B76:E76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>